<commit_message>
model wetland updates - kw
</commit_message>
<xml_diff>
--- a/Wetlands/Methane_worksheet_FINAL.xlsx
+++ b/Wetlands/Methane_worksheet_FINAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Wetlands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56463156-8CD6-4A40-86D3-01725EE11FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A285C3B-06A8-2342-8913-5E2223ABC2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="960" windowWidth="33600" windowHeight="17540" xr2:uid="{E7E559FF-5818-C841-AE4A-F705F0A80E92}"/>
   </bookViews>
@@ -743,6 +743,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -752,10 +756,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,10 +864,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1169,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B10BDFC-C098-7F4B-8D19-0A28C207B653}">
   <dimension ref="A1:BE780"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1208,7 +1204,7 @@
       </c>
       <c r="N1" s="22"/>
       <c r="O1" s="23"/>
-      <c r="T1" s="52"/>
+      <c r="T1" s="49"/>
     </row>
     <row r="2" spans="1:57" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1221,7 +1217,7 @@
       <c r="L2" s="4"/>
       <c r="N2" s="12"/>
       <c r="O2" s="4"/>
-      <c r="T2" s="53"/>
+      <c r="T2" s="50"/>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1236,7 +1232,7 @@
       </c>
       <c r="L3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="T3" s="53"/>
+      <c r="T3" s="50"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1252,7 +1248,7 @@
       <c r="L4" s="4"/>
       <c r="O4" s="4"/>
       <c r="R4" s="27"/>
-      <c r="T4" s="53"/>
+      <c r="T4" s="50"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1267,7 +1263,7 @@
       <c r="I5" s="4"/>
       <c r="L5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="T5" s="53"/>
+      <c r="T5" s="50"/>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1284,7 +1280,7 @@
       <c r="L6" s="4"/>
       <c r="N6" s="8"/>
       <c r="O6" s="4"/>
-      <c r="T6" s="54" t="s">
+      <c r="T6" s="51" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1307,7 +1303,7 @@
       <c r="L7" s="4"/>
       <c r="O7" s="4"/>
       <c r="Q7" s="27"/>
-      <c r="T7" s="53" t="s">
+      <c r="T7" s="50" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1322,7 +1318,7 @@
       <c r="O8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T8" s="53"/>
+      <c r="T8" s="50"/>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1346,7 +1342,7 @@
       <c r="O9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="T9" s="53"/>
+      <c r="T9" s="50"/>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.2">
       <c r="I10" s="4"/>
@@ -1357,7 +1353,7 @@
         <v>26</v>
       </c>
       <c r="O10" s="4"/>
-      <c r="T10" s="53"/>
+      <c r="T10" s="50"/>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1370,12 +1366,12 @@
       <c r="I11" s="4"/>
       <c r="L11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="T11" s="53"/>
+      <c r="T11" s="50"/>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.2">
       <c r="I12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="T12" s="55"/>
+      <c r="T12" s="52"/>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A13" s="45"/>
@@ -1395,13 +1391,13 @@
         <v>37</v>
       </c>
       <c r="O13" s="17"/>
-      <c r="P13" s="50" t="s">
+      <c r="P13" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="51"/>
+      <c r="Q13" s="55"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="55"/>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A14" s="45"/>
@@ -1425,14 +1421,14 @@
         <v>77</v>
       </c>
       <c r="O14" s="17"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="49"/>
-      <c r="V14" s="49"/>
-      <c r="W14" s="49"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="55"/>
+      <c r="S14" s="55"/>
+      <c r="T14" s="55"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53"/>
+      <c r="W14" s="53"/>
       <c r="X14" s="28"/>
       <c r="Y14" s="28"/>
       <c r="Z14" s="28"/>
@@ -1710,11 +1706,11 @@
         <v>62.748750000000001</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" ref="O18:O81" si="4">$N$8*EXP($N$9*(1/(M18+$B$3)-1/298.15))</f>
+        <f>$N$8*EXP($N$9*(1/(M18+$B$3)-1/298.15))</f>
         <v>2.0365175140760038E-3</v>
       </c>
       <c r="P18" s="3">
-        <f t="shared" ref="P18:P81" si="5">L18*$B$2*($B$5+$B$3)</f>
+        <f t="shared" ref="P18:P81" si="4">L18*$B$2*($B$5+$B$3)</f>
         <v>583.62628181546143</v>
       </c>
       <c r="Q18" s="33">
@@ -1726,7 +1722,7 @@
         <v>1.1845999746421498</v>
       </c>
       <c r="S18" s="3">
-        <f t="shared" ref="S18:S81" si="6">O18*10^6*R18/10^6</f>
+        <f t="shared" ref="S18:S81" si="5">O18*10^6*R18/10^6</f>
         <v>2.4124585955327283E-3</v>
       </c>
       <c r="T18" s="33">
@@ -1785,15 +1781,15 @@
         <v>62.602290000000004</v>
       </c>
       <c r="O19" s="5">
+        <f t="shared" ref="O18:O81" si="6">$N$8*EXP($N$9*(1/(M19+$B$3)-1/298.15))</f>
+        <v>2.0614974303226059E-3</v>
+      </c>
+      <c r="P19" s="3">
         <f t="shared" si="4"/>
-        <v>2.0614974303226059E-3</v>
-      </c>
-      <c r="P19" s="3">
-        <f t="shared" si="5"/>
         <v>16.189874724844724</v>
       </c>
       <c r="Q19" s="33">
-        <f t="shared" ref="Q18:Q81" si="7">((L19*H19/1000)+(I19*O19*P19))/I19</f>
+        <f t="shared" ref="Q19:Q81" si="7">((L19*H19/1000)+(I19*O19*P19))/I19</f>
         <v>0.21208171146196489</v>
       </c>
       <c r="R19" s="3">
@@ -1801,7 +1797,7 @@
         <v>1.1818350349057236</v>
       </c>
       <c r="S19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4363498875233764E-3</v>
       </c>
       <c r="T19" s="33">
@@ -1860,11 +1856,11 @@
         <v>61.669130000000003</v>
       </c>
       <c r="O20" s="5">
+        <f t="shared" si="6"/>
+        <v>2.1178799437077682E-3</v>
+      </c>
+      <c r="P20" s="3">
         <f t="shared" si="4"/>
-        <v>2.1178799437077682E-3</v>
-      </c>
-      <c r="P20" s="3">
-        <f t="shared" si="5"/>
         <v>4.5888093250059452</v>
       </c>
       <c r="Q20" s="33">
@@ -1876,7 +1872,7 @@
         <v>1.1642184080830844</v>
       </c>
       <c r="S20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4656748165745503E-3</v>
       </c>
       <c r="T20" s="33">
@@ -1935,11 +1931,11 @@
         <v>62.602290000000004</v>
       </c>
       <c r="O21" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0614974303226059E-3</v>
+      </c>
+      <c r="P21" s="3">
         <f t="shared" si="4"/>
-        <v>2.0614974303226059E-3</v>
-      </c>
-      <c r="P21" s="3">
-        <f t="shared" si="5"/>
         <v>32.7968643657576</v>
       </c>
       <c r="Q21" s="33">
@@ -1955,7 +1951,7 @@
         <v>2.4363498875233764E-3</v>
       </c>
       <c r="T21" s="33">
-        <f t="shared" ref="T20:T81" si="9">Q21/S21*100</f>
+        <f t="shared" ref="T21:T81" si="9">Q21/S21*100</f>
         <v>17900.026002828912</v>
       </c>
       <c r="U21" s="3"/>
@@ -2010,11 +2006,11 @@
         <v>64.56</v>
       </c>
       <c r="O22" s="5">
+        <f t="shared" si="6"/>
+        <v>1.999880935237024E-3</v>
+      </c>
+      <c r="P22" s="3">
         <f t="shared" si="4"/>
-        <v>1.999880935237024E-3</v>
-      </c>
-      <c r="P22" s="3">
-        <f t="shared" si="5"/>
         <v>65.505216764576119</v>
       </c>
       <c r="Q22" s="33">
@@ -2026,7 +2022,7 @@
         <v>1.2187935913129297</v>
       </c>
       <c r="S22" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4374420672557931E-3</v>
       </c>
       <c r="T22" s="33">
@@ -2085,11 +2081,11 @@
         <v>61.907879999999999</v>
       </c>
       <c r="O23" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0416382657432999E-3</v>
+      </c>
+      <c r="P23" s="3">
         <f t="shared" si="4"/>
-        <v>2.0416382657432999E-3</v>
-      </c>
-      <c r="P23" s="3">
-        <f t="shared" si="5"/>
         <v>6.0655233524803318</v>
       </c>
       <c r="Q23" s="33">
@@ -2101,7 +2097,7 @@
         <v>1.1687256411984184</v>
       </c>
       <c r="S23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3861149912260647E-3</v>
       </c>
       <c r="T23" s="33">
@@ -2160,11 +2156,11 @@
         <v>61.669130000000003</v>
       </c>
       <c r="O24" s="5">
+        <f t="shared" si="6"/>
+        <v>2.1178799437077682E-3</v>
+      </c>
+      <c r="P24" s="3">
         <f t="shared" si="4"/>
-        <v>2.1178799437077682E-3</v>
-      </c>
-      <c r="P24" s="3">
-        <f t="shared" si="5"/>
         <v>3.435791012353945</v>
       </c>
       <c r="Q24" s="33">
@@ -2176,7 +2172,7 @@
         <v>1.1642184080830844</v>
       </c>
       <c r="S24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4656748165745503E-3</v>
       </c>
       <c r="T24" s="33">
@@ -2235,11 +2231,11 @@
         <v>62.682319999999997</v>
       </c>
       <c r="O25" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0280213654239017E-3</v>
+      </c>
+      <c r="P25" s="3">
         <f t="shared" si="4"/>
-        <v>2.0280213654239017E-3</v>
-      </c>
-      <c r="P25" s="3">
-        <f t="shared" si="5"/>
         <v>67.489920417501693</v>
       </c>
       <c r="Q25" s="33">
@@ -2251,7 +2247,7 @@
         <v>1.1833458783244466</v>
       </c>
       <c r="S25" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3998507239282904E-3</v>
       </c>
       <c r="T25" s="33">
@@ -2310,11 +2306,11 @@
         <v>62.682319999999997</v>
       </c>
       <c r="O26" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0280213654239017E-3</v>
+      </c>
+      <c r="P26" s="3">
         <f t="shared" si="4"/>
-        <v>2.0280213654239017E-3</v>
-      </c>
-      <c r="P26" s="3">
-        <f t="shared" si="5"/>
         <v>35.605983382206098</v>
       </c>
       <c r="Q26" s="33">
@@ -2326,7 +2322,7 @@
         <v>1.1833458783244466</v>
       </c>
       <c r="S26" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3998507239282904E-3</v>
       </c>
       <c r="T26" s="33">
@@ -2385,11 +2381,11 @@
         <v>63.841279999999998</v>
       </c>
       <c r="O27" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9988624233304225E-3</v>
+      </c>
+      <c r="P27" s="3">
         <f t="shared" si="4"/>
-        <v>1.9988624233304225E-3</v>
-      </c>
-      <c r="P27" s="3">
-        <f t="shared" si="5"/>
         <v>69.982795445297228</v>
       </c>
       <c r="Q27" s="33">
@@ -2401,7 +2397,7 @@
         <v>1.2052252621625512</v>
       </c>
       <c r="S27" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4090794881852806E-3</v>
       </c>
       <c r="T27" s="33">
@@ -2460,11 +2456,11 @@
         <v>62.682319999999997</v>
       </c>
       <c r="O28" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0280213654239017E-3</v>
+      </c>
+      <c r="P28" s="3">
         <f t="shared" si="4"/>
-        <v>2.0280213654239017E-3</v>
-      </c>
-      <c r="P28" s="3">
-        <f t="shared" si="5"/>
         <v>15.906345631569643</v>
       </c>
       <c r="Q28" s="33">
@@ -2476,7 +2472,7 @@
         <v>1.1833458783244466</v>
       </c>
       <c r="S28" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3998507239282904E-3</v>
       </c>
       <c r="T28" s="33">
@@ -2535,11 +2531,11 @@
         <v>63.809089999999998</v>
       </c>
       <c r="O29" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9785179564049708E-3</v>
+      </c>
+      <c r="P29" s="3">
         <f t="shared" si="4"/>
-        <v>1.9785179564049708E-3</v>
-      </c>
-      <c r="P29" s="3">
-        <f t="shared" si="5"/>
         <v>881.42779344740609</v>
       </c>
       <c r="Q29" s="33">
@@ -2551,7 +2547,7 @@
         <v>1.2046175644285926</v>
       </c>
       <c r="S29" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3833574818227922E-3</v>
       </c>
       <c r="T29" s="33">
@@ -2610,11 +2606,11 @@
         <v>63.841279999999998</v>
       </c>
       <c r="O30" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9988624233304225E-3</v>
+      </c>
+      <c r="P30" s="3">
         <f t="shared" si="4"/>
-        <v>1.9988624233304225E-3</v>
-      </c>
-      <c r="P30" s="3">
-        <f t="shared" si="5"/>
         <v>153.24438517506292</v>
       </c>
       <c r="Q30" s="33">
@@ -2626,7 +2622,7 @@
         <v>1.2052252621625512</v>
       </c>
       <c r="S30" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4090794881852806E-3</v>
       </c>
       <c r="T30" s="33">
@@ -2685,11 +2681,11 @@
         <v>62.784979999999997</v>
       </c>
       <c r="O31" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9459632108846249E-3</v>
+      </c>
+      <c r="P31" s="3">
         <f t="shared" si="4"/>
-        <v>1.9459632108846249E-3</v>
-      </c>
-      <c r="P31" s="3">
-        <f t="shared" si="5"/>
         <v>27.025956821097083</v>
       </c>
       <c r="Q31" s="33">
@@ -2701,7 +2697,7 @@
         <v>1.185283941367882</v>
       </c>
       <c r="S31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3065189443542272E-3</v>
       </c>
       <c r="T31" s="33">
@@ -2760,11 +2756,11 @@
         <v>63.841279999999998</v>
       </c>
       <c r="O32" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9988624233304225E-3</v>
+      </c>
+      <c r="P32" s="3">
         <f t="shared" si="4"/>
-        <v>1.9988624233304225E-3</v>
-      </c>
-      <c r="P32" s="3">
-        <f t="shared" si="5"/>
         <v>63.418006439466467</v>
       </c>
       <c r="Q32" s="33">
@@ -2776,7 +2772,7 @@
         <v>1.2052252621625512</v>
       </c>
       <c r="S32" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4090794881852806E-3</v>
       </c>
       <c r="T32" s="33">
@@ -2835,11 +2831,11 @@
         <v>61.907879999999999</v>
       </c>
       <c r="O33" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0416382657432999E-3</v>
+      </c>
+      <c r="P33" s="3">
         <f t="shared" si="4"/>
-        <v>2.0416382657432999E-3</v>
-      </c>
-      <c r="P33" s="3">
-        <f t="shared" si="5"/>
         <v>6.204925156673915</v>
       </c>
       <c r="Q33" s="33">
@@ -2851,7 +2847,7 @@
         <v>1.1687256411984184</v>
       </c>
       <c r="S33" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3861149912260647E-3</v>
       </c>
       <c r="T33" s="33">
@@ -2910,11 +2906,11 @@
         <v>61.64864</v>
       </c>
       <c r="O34" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0844166189658169E-3</v>
+      </c>
+      <c r="P34" s="3">
         <f t="shared" si="4"/>
-        <v>2.0844166189658169E-3</v>
-      </c>
-      <c r="P34" s="3">
-        <f t="shared" si="5"/>
         <v>2.7765858704893791</v>
       </c>
       <c r="Q34" s="33">
@@ -2926,7 +2922,7 @@
         <v>1.1638315883698565</v>
       </c>
       <c r="S34" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4259099044755122E-3</v>
       </c>
       <c r="T34" s="33">
@@ -2985,11 +2981,11 @@
         <v>62.682319999999997</v>
       </c>
       <c r="O35" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0280213654239017E-3</v>
+      </c>
+      <c r="P35" s="3">
         <f t="shared" si="4"/>
-        <v>2.0280213654239017E-3</v>
-      </c>
-      <c r="P35" s="3">
-        <f t="shared" si="5"/>
         <v>58.556572986311409</v>
       </c>
       <c r="Q35" s="33">
@@ -3001,7 +2997,7 @@
         <v>1.1833458783244466</v>
       </c>
       <c r="S35" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3998507239282904E-3</v>
       </c>
       <c r="T35" s="33">
@@ -3060,11 +3056,11 @@
         <v>61.64864</v>
       </c>
       <c r="O36" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0844166189658169E-3</v>
+      </c>
+      <c r="P36" s="3">
         <f t="shared" si="4"/>
-        <v>2.0844166189658169E-3</v>
-      </c>
-      <c r="P36" s="3">
-        <f t="shared" si="5"/>
         <v>3.3011146930482811</v>
       </c>
       <c r="Q36" s="33">
@@ -3076,7 +3072,7 @@
         <v>1.1638315883698565</v>
       </c>
       <c r="S36" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4259099044755122E-3</v>
       </c>
       <c r="T36" s="33">
@@ -3135,11 +3131,11 @@
         <v>62.492400000000004</v>
       </c>
       <c r="O37" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9809541385858932E-3</v>
+      </c>
+      <c r="P37" s="3">
         <f t="shared" si="4"/>
-        <v>1.9809541385858932E-3</v>
-      </c>
-      <c r="P37" s="3">
-        <f t="shared" si="5"/>
         <v>158.51802630997943</v>
       </c>
       <c r="Q37" s="33">
@@ -3151,7 +3147,7 @@
         <v>1.1797604805725546</v>
       </c>
       <c r="S37" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.337051406530284E-3</v>
       </c>
       <c r="T37" s="33">
@@ -3210,11 +3206,11 @@
         <v>61.903919999999999</v>
       </c>
       <c r="O38" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9947791269277924E-3</v>
+      </c>
+      <c r="P38" s="3">
         <f t="shared" si="4"/>
-        <v>1.9947791269277924E-3</v>
-      </c>
-      <c r="P38" s="3">
-        <f t="shared" si="5"/>
         <v>5.7134747283304383</v>
       </c>
       <c r="Q38" s="33">
@@ -3226,7 +3222,7 @@
         <v>1.1686508824837096</v>
       </c>
       <c r="S38" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3312003870442485E-3</v>
       </c>
       <c r="T38" s="33">
@@ -3285,11 +3281,11 @@
         <v>61.903919999999999</v>
       </c>
       <c r="O39" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9947791269277924E-3</v>
+      </c>
+      <c r="P39" s="3">
         <f t="shared" si="4"/>
-        <v>1.9947791269277924E-3</v>
-      </c>
-      <c r="P39" s="3">
-        <f t="shared" si="5"/>
         <v>5.0022892526987741</v>
       </c>
       <c r="Q39" s="33">
@@ -3301,7 +3297,7 @@
         <v>1.1686508824837096</v>
       </c>
       <c r="S39" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3312003870442485E-3</v>
       </c>
       <c r="T39" s="33">
@@ -3360,11 +3356,11 @@
         <v>61.709899999999998</v>
       </c>
       <c r="O40" s="5">
+        <f t="shared" si="6"/>
+        <v>2.1041761578601799E-3</v>
+      </c>
+      <c r="P40" s="3">
         <f t="shared" si="4"/>
-        <v>2.1041761578601799E-3</v>
-      </c>
-      <c r="P40" s="3">
-        <f t="shared" si="5"/>
         <v>3.1073698126436415</v>
       </c>
       <c r="Q40" s="33">
@@ -3376,7 +3372,7 @@
         <v>1.1649880830322454</v>
       </c>
       <c r="S40" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4513401485076864E-3</v>
       </c>
       <c r="T40" s="33">
@@ -3435,11 +3431,11 @@
         <v>63.79533</v>
       </c>
       <c r="O41" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9866139527056686E-3</v>
+      </c>
+      <c r="P41" s="3">
         <f t="shared" si="4"/>
-        <v>1.9866139527056686E-3</v>
-      </c>
-      <c r="P41" s="3">
-        <f t="shared" si="5"/>
         <v>39.041047396884984</v>
       </c>
       <c r="Q41" s="33">
@@ -3451,7 +3447,7 @@
         <v>1.2043577967734431</v>
       </c>
       <c r="S41" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3925940031199805E-3</v>
       </c>
       <c r="T41" s="33">
@@ -3510,11 +3506,11 @@
         <v>62.77</v>
       </c>
       <c r="O42" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0269419612688765E-3</v>
+      </c>
+      <c r="P42" s="3">
         <f t="shared" si="4"/>
-        <v>2.0269419612688765E-3</v>
-      </c>
-      <c r="P42" s="3">
-        <f t="shared" si="5"/>
         <v>39.041047396884984</v>
       </c>
       <c r="Q42" s="33">
@@ -3526,7 +3522,7 @@
         <v>1.1850011419874937</v>
       </c>
       <c r="S42" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4019285388459889E-3</v>
       </c>
       <c r="T42" s="33">
@@ -3585,11 +3581,11 @@
         <v>63.79533</v>
       </c>
       <c r="O43" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9866139527056686E-3</v>
+      </c>
+      <c r="P43" s="3">
         <f t="shared" si="4"/>
-        <v>1.9866139527056686E-3</v>
-      </c>
-      <c r="P43" s="3">
-        <f t="shared" si="5"/>
         <v>604.03165255916656</v>
       </c>
       <c r="Q43" s="33">
@@ -3601,7 +3597,7 @@
         <v>1.2043577967734431</v>
       </c>
       <c r="S43" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3925940031199805E-3</v>
       </c>
       <c r="T43" s="33">
@@ -3660,11 +3656,11 @@
         <v>63.775939999999999</v>
       </c>
       <c r="O44" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9506684189233771E-3</v>
+      </c>
+      <c r="P44" s="3">
         <f t="shared" si="4"/>
-        <v>1.9506684189233771E-3</v>
-      </c>
-      <c r="P44" s="3">
-        <f t="shared" si="5"/>
         <v>858.98755621119597</v>
       </c>
       <c r="Q44" s="33">
@@ -3676,7 +3672,7 @@
         <v>1.2039917433698564</v>
       </c>
       <c r="S44" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3485886704360782E-3</v>
       </c>
       <c r="T44" s="33">
@@ -3735,11 +3731,11 @@
         <v>63.28</v>
       </c>
       <c r="O45" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9886752759355397E-3</v>
+      </c>
+      <c r="P45" s="3">
         <f t="shared" si="4"/>
-        <v>1.9886752759355397E-3</v>
-      </c>
-      <c r="P45" s="3">
-        <f t="shared" si="5"/>
         <v>48.342982649332875</v>
       </c>
       <c r="Q45" s="33">
@@ -3751,7 +3747,7 @@
         <v>1.1946291582757465</v>
       </c>
       <c r="S45" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3757294709746616E-3</v>
       </c>
       <c r="T45" s="33">
@@ -3810,11 +3806,11 @@
         <v>61.903919999999999</v>
       </c>
       <c r="O46" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9947791269277924E-3</v>
+      </c>
+      <c r="P46" s="3">
         <f t="shared" si="4"/>
-        <v>1.9947791269277924E-3</v>
-      </c>
-      <c r="P46" s="3">
-        <f t="shared" si="5"/>
         <v>5.8079844260887992</v>
       </c>
       <c r="Q46" s="33">
@@ -3826,7 +3822,7 @@
         <v>1.1686508824837096</v>
       </c>
       <c r="S46" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3312003870442485E-3</v>
       </c>
       <c r="T46" s="33">
@@ -3885,11 +3881,11 @@
         <v>62.853400000000001</v>
       </c>
       <c r="O47" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0062850491605233E-3</v>
+      </c>
+      <c r="P47" s="3">
         <f t="shared" si="4"/>
-        <v>2.0062850491605233E-3</v>
-      </c>
-      <c r="P47" s="3">
-        <f t="shared" si="5"/>
         <v>89.389271383463992</v>
       </c>
       <c r="Q47" s="33">
@@ -3901,7 +3897,7 @@
         <v>1.1865756058275727</v>
       </c>
       <c r="S47" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3806088976704495E-3</v>
       </c>
       <c r="T47" s="33">
@@ -3960,11 +3956,11 @@
         <v>62.492400000000004</v>
       </c>
       <c r="O48" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9809541385858932E-3</v>
+      </c>
+      <c r="P48" s="3">
         <f t="shared" si="4"/>
-        <v>1.9809541385858932E-3</v>
-      </c>
-      <c r="P48" s="3">
-        <f t="shared" si="5"/>
         <v>157.93133918620254</v>
       </c>
       <c r="Q48" s="33">
@@ -3976,7 +3972,7 @@
         <v>1.1797604805725546</v>
       </c>
       <c r="S48" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.337051406530284E-3</v>
       </c>
       <c r="T48" s="33">
@@ -4035,11 +4031,11 @@
         <v>62.853400000000001</v>
       </c>
       <c r="O49" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0062850491605233E-3</v>
+      </c>
+      <c r="P49" s="3">
         <f t="shared" si="4"/>
-        <v>2.0062850491605233E-3</v>
-      </c>
-      <c r="P49" s="3">
-        <f t="shared" si="5"/>
         <v>98.180854268016759</v>
       </c>
       <c r="Q49" s="33">
@@ -4051,7 +4047,7 @@
         <v>1.1865756058275727</v>
       </c>
       <c r="S49" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3806088976704495E-3</v>
       </c>
       <c r="T49" s="33">
@@ -4110,11 +4106,11 @@
         <v>64.56</v>
       </c>
       <c r="O50" s="5">
+        <f t="shared" si="6"/>
+        <v>1.999880935237024E-3</v>
+      </c>
+      <c r="P50" s="3">
         <f t="shared" si="4"/>
-        <v>1.999880935237024E-3</v>
-      </c>
-      <c r="P50" s="3">
-        <f t="shared" si="5"/>
         <v>68.763620344214374</v>
       </c>
       <c r="Q50" s="33">
@@ -4126,7 +4122,7 @@
         <v>1.2187935913129297</v>
       </c>
       <c r="S50" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4374420672557931E-3</v>
       </c>
       <c r="T50" s="33">
@@ -4185,11 +4181,11 @@
         <v>64.56</v>
       </c>
       <c r="O51" s="5">
+        <f t="shared" si="6"/>
+        <v>1.999880935237024E-3</v>
+      </c>
+      <c r="P51" s="3">
         <f t="shared" si="4"/>
-        <v>1.999880935237024E-3</v>
-      </c>
-      <c r="P51" s="3">
-        <f t="shared" si="5"/>
         <v>66.80290761456591</v>
       </c>
       <c r="Q51" s="33">
@@ -4201,7 +4197,7 @@
         <v>1.2187935913129297</v>
       </c>
       <c r="S51" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4374420672557931E-3</v>
       </c>
       <c r="T51" s="33">
@@ -4260,11 +4256,11 @@
         <v>62.413539999999998</v>
       </c>
       <c r="O52" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0459188357933003E-3</v>
+      </c>
+      <c r="P52" s="3">
         <f t="shared" si="4"/>
-        <v>2.0459188357933003E-3</v>
-      </c>
-      <c r="P52" s="3">
-        <f t="shared" si="5"/>
         <v>80.597688498911268</v>
       </c>
       <c r="Q52" s="33">
@@ -4276,7 +4272,7 @@
         <v>1.1782717249559043</v>
       </c>
       <c r="S52" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4106483157699471E-3</v>
       </c>
       <c r="T52" s="33">
@@ -4335,11 +4331,11 @@
         <v>62.413539999999998</v>
       </c>
       <c r="O53" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0459188357933003E-3</v>
+      </c>
+      <c r="P53" s="3">
         <f t="shared" si="4"/>
-        <v>2.0459188357933003E-3</v>
-      </c>
-      <c r="P53" s="3">
-        <f t="shared" si="5"/>
         <v>66.669867040029146</v>
       </c>
       <c r="Q53" s="33">
@@ -4351,7 +4347,7 @@
         <v>1.1782717249559043</v>
       </c>
       <c r="S53" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4106483157699471E-3</v>
       </c>
       <c r="T53" s="33">
@@ -4410,11 +4406,11 @@
         <v>62.413539999999998</v>
       </c>
       <c r="O54" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0459188357933003E-3</v>
+      </c>
+      <c r="P54" s="3">
         <f t="shared" si="4"/>
-        <v>2.0459188357933003E-3</v>
-      </c>
-      <c r="P54" s="3">
-        <f t="shared" si="5"/>
         <v>67.640408936240007</v>
       </c>
       <c r="Q54" s="33">
@@ -4426,7 +4422,7 @@
         <v>1.1782717249559043</v>
       </c>
       <c r="S54" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4106483157699471E-3</v>
       </c>
       <c r="T54" s="33">
@@ -4485,11 +4481,11 @@
         <v>62.413539999999998</v>
       </c>
       <c r="O55" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0459188357933003E-3</v>
+      </c>
+      <c r="P55" s="3">
         <f t="shared" si="4"/>
-        <v>2.0459188357933003E-3</v>
-      </c>
-      <c r="P55" s="3">
-        <f t="shared" si="5"/>
         <v>73.34806768316993</v>
       </c>
       <c r="Q55" s="33">
@@ -4501,7 +4497,7 @@
         <v>1.1782717249559043</v>
       </c>
       <c r="S55" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4106483157699471E-3</v>
       </c>
       <c r="T55" s="33">
@@ -4560,11 +4556,11 @@
         <v>62.965649999999997</v>
       </c>
       <c r="O56" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9904883909304654E-3</v>
+      </c>
+      <c r="P56" s="3">
         <f t="shared" si="4"/>
-        <v>1.9904883909304654E-3</v>
-      </c>
-      <c r="P56" s="3">
-        <f t="shared" si="5"/>
         <v>29.479573974439141</v>
       </c>
       <c r="Q56" s="33">
@@ -4576,7 +4572,7 @@
         <v>1.1886947133341537</v>
       </c>
       <c r="S56" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3660830272520502E-3</v>
       </c>
       <c r="T56" s="33">
@@ -4635,11 +4631,11 @@
         <v>63.79533</v>
       </c>
       <c r="O57" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9866139527056686E-3</v>
+      </c>
+      <c r="P57" s="3">
         <f t="shared" si="4"/>
-        <v>1.9866139527056686E-3</v>
-      </c>
-      <c r="P57" s="3">
-        <f t="shared" si="5"/>
         <v>466.1601784715948</v>
       </c>
       <c r="Q57" s="33">
@@ -4651,7 +4647,7 @@
         <v>1.2043577967734431</v>
       </c>
       <c r="S57" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3925940031199805E-3</v>
       </c>
       <c r="T57" s="33">
@@ -4710,11 +4706,11 @@
         <v>62.965649999999997</v>
       </c>
       <c r="O58" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9904883909304654E-3</v>
+      </c>
+      <c r="P58" s="3">
         <f t="shared" si="4"/>
-        <v>1.9904883909304654E-3</v>
-      </c>
-      <c r="P58" s="3">
-        <f t="shared" si="5"/>
         <v>38.700812484954888</v>
       </c>
       <c r="Q58" s="33">
@@ -4726,7 +4722,7 @@
         <v>1.1886947133341537</v>
       </c>
       <c r="S58" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3660830272520502E-3</v>
       </c>
       <c r="T58" s="33">
@@ -4785,11 +4781,11 @@
         <v>63.775939999999999</v>
       </c>
       <c r="O59" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9506684189233771E-3</v>
+      </c>
+      <c r="P59" s="3">
         <f t="shared" si="4"/>
-        <v>1.9506684189233771E-3</v>
-      </c>
-      <c r="P59" s="3">
-        <f t="shared" si="5"/>
         <v>677.87135242009867</v>
       </c>
       <c r="Q59" s="33">
@@ -4801,7 +4797,7 @@
         <v>1.2039917433698564</v>
       </c>
       <c r="S59" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3485886704360782E-3</v>
       </c>
       <c r="T59" s="33">
@@ -4860,11 +4856,11 @@
         <v>62.965649999999997</v>
       </c>
       <c r="O60" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9904883909304654E-3</v>
+      </c>
+      <c r="P60" s="3">
         <f t="shared" si="4"/>
-        <v>1.9904883909304654E-3</v>
-      </c>
-      <c r="P60" s="3">
-        <f t="shared" si="5"/>
         <v>23.4992910993601</v>
       </c>
       <c r="Q60" s="33">
@@ -4876,7 +4872,7 @@
         <v>1.1886947133341537</v>
       </c>
       <c r="S60" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3660830272520502E-3</v>
       </c>
       <c r="T60" s="33">
@@ -4935,11 +4931,11 @@
         <v>62.965649999999997</v>
       </c>
       <c r="O61" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9904883909304654E-3</v>
+      </c>
+      <c r="P61" s="3">
         <f t="shared" si="4"/>
-        <v>1.9904883909304654E-3</v>
-      </c>
-      <c r="P61" s="3">
-        <f t="shared" si="5"/>
         <v>42.517550279042531</v>
       </c>
       <c r="Q61" s="33">
@@ -4951,7 +4947,7 @@
         <v>1.1886947133341537</v>
       </c>
       <c r="S61" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3660830272520502E-3</v>
       </c>
       <c r="T61" s="33">
@@ -5010,11 +5006,11 @@
         <v>63.784350000000003</v>
       </c>
       <c r="O62" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9988624233304225E-3</v>
+      </c>
+      <c r="P62" s="3">
         <f t="shared" si="4"/>
-        <v>1.9988624233304225E-3</v>
-      </c>
-      <c r="P62" s="3">
-        <f t="shared" si="5"/>
         <v>188.62663502276797</v>
       </c>
       <c r="Q62" s="33">
@@ -5026,7 +5022,7 @@
         <v>1.204150511246296</v>
       </c>
       <c r="S62" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4069312089643382E-3</v>
       </c>
       <c r="T62" s="33">
@@ -5085,11 +5081,11 @@
         <v>61.64864</v>
       </c>
       <c r="O63" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0844166189658169E-3</v>
+      </c>
+      <c r="P63" s="3">
         <f t="shared" si="4"/>
-        <v>2.0844166189658169E-3</v>
-      </c>
-      <c r="P63" s="3">
-        <f t="shared" si="5"/>
         <v>3.2255069348415919</v>
       </c>
       <c r="Q63" s="33">
@@ -5101,7 +5097,7 @@
         <v>1.1638315883698565</v>
       </c>
       <c r="S63" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4259099044755122E-3</v>
       </c>
       <c r="T63" s="33">
@@ -5160,11 +5156,11 @@
         <v>62.492400000000004</v>
       </c>
       <c r="O64" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9809541385858932E-3</v>
+      </c>
+      <c r="P64" s="3">
         <f t="shared" si="4"/>
-        <v>1.9809541385858932E-3</v>
-      </c>
-      <c r="P64" s="3">
-        <f t="shared" si="5"/>
         <v>155.2530797512656</v>
       </c>
       <c r="Q64" s="33">
@@ -5176,7 +5172,7 @@
         <v>1.1797604805725546</v>
       </c>
       <c r="S64" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.337051406530284E-3</v>
       </c>
       <c r="T64" s="33">
@@ -5235,11 +5231,11 @@
         <v>62.4</v>
       </c>
       <c r="O65" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0931031059290566E-3</v>
+      </c>
+      <c r="P65" s="3">
         <f t="shared" si="4"/>
-        <v>2.0931031059290566E-3</v>
-      </c>
-      <c r="P65" s="3">
-        <f t="shared" si="5"/>
         <v>52.816199344003593</v>
       </c>
       <c r="Q65" s="33">
@@ -5251,7 +5247,7 @@
         <v>1.178016110562683</v>
       </c>
       <c r="S65" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4657091798532186E-3</v>
       </c>
       <c r="T65" s="33">
@@ -5310,11 +5306,11 @@
         <v>61.709899999999998</v>
       </c>
       <c r="O66" s="5">
+        <f t="shared" si="6"/>
+        <v>2.1041761578601799E-3</v>
+      </c>
+      <c r="P66" s="3">
         <f t="shared" si="4"/>
-        <v>2.1041761578601799E-3</v>
-      </c>
-      <c r="P66" s="3">
-        <f t="shared" si="5"/>
         <v>3.1357227219711499</v>
       </c>
       <c r="Q66" s="33">
@@ -5326,7 +5322,7 @@
         <v>1.1649880830322454</v>
       </c>
       <c r="S66" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4513401485076864E-3</v>
       </c>
       <c r="T66" s="33">
@@ -5385,11 +5381,11 @@
         <v>62.748750000000001</v>
       </c>
       <c r="O67" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0365175140760038E-3</v>
+      </c>
+      <c r="P67" s="3">
         <f t="shared" si="4"/>
-        <v>2.0365175140760038E-3</v>
-      </c>
-      <c r="P67" s="3">
-        <f t="shared" si="5"/>
         <v>31.488268550641838</v>
       </c>
       <c r="Q67" s="33">
@@ -5401,7 +5397,7 @@
         <v>1.1845999746421498</v>
       </c>
       <c r="S67" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4124585955327283E-3</v>
       </c>
       <c r="T67" s="33">
@@ -5460,11 +5456,11 @@
         <v>61.709899999999998</v>
       </c>
       <c r="O68" s="5">
+        <f t="shared" si="6"/>
+        <v>2.1041761578601799E-3</v>
+      </c>
+      <c r="P68" s="3">
         <f t="shared" si="4"/>
-        <v>2.1041761578601799E-3</v>
-      </c>
-      <c r="P68" s="3">
-        <f t="shared" si="5"/>
         <v>3.0931933579798874</v>
       </c>
       <c r="Q68" s="33">
@@ -5476,7 +5472,7 @@
         <v>1.1649880830322454</v>
       </c>
       <c r="S68" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4513401485076864E-3</v>
       </c>
       <c r="T68" s="33">
@@ -5535,11 +5531,11 @@
         <v>63.28</v>
       </c>
       <c r="O69" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9886752759355397E-3</v>
+      </c>
+      <c r="P69" s="3">
         <f t="shared" si="4"/>
-        <v>1.9886752759355397E-3</v>
-      </c>
-      <c r="P69" s="3">
-        <f t="shared" si="5"/>
         <v>67.2761831010328</v>
       </c>
       <c r="Q69" s="33">
@@ -5551,7 +5547,7 @@
         <v>1.1946291582757465</v>
       </c>
       <c r="S69" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3757294709746616E-3</v>
       </c>
       <c r="T69" s="33">
@@ -5610,11 +5606,11 @@
         <v>63.841279999999998</v>
       </c>
       <c r="O70" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9988624233304225E-3</v>
+      </c>
+      <c r="P70" s="3">
         <f t="shared" si="4"/>
-        <v>1.9988624233304225E-3</v>
-      </c>
-      <c r="P70" s="3">
-        <f t="shared" si="5"/>
         <v>74.0656143884584</v>
       </c>
       <c r="Q70" s="33">
@@ -5626,7 +5622,7 @@
         <v>1.2052252621625512</v>
       </c>
       <c r="S70" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4090794881852806E-3</v>
       </c>
       <c r="T70" s="33">
@@ -5685,11 +5681,11 @@
         <v>63.79533</v>
       </c>
       <c r="O71" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9866139527056686E-3</v>
+      </c>
+      <c r="P71" s="3">
         <f t="shared" si="4"/>
-        <v>1.9866139527056686E-3</v>
-      </c>
-      <c r="P71" s="3">
-        <f t="shared" si="5"/>
         <v>340.88175811148716</v>
       </c>
       <c r="Q71" s="33">
@@ -5701,7 +5697,7 @@
         <v>1.2043577967734431</v>
       </c>
       <c r="S71" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3925940031199805E-3</v>
       </c>
       <c r="T71" s="33">
@@ -5760,11 +5756,11 @@
         <v>62.4</v>
       </c>
       <c r="O72" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0931031059290566E-3</v>
+      </c>
+      <c r="P72" s="3">
         <f t="shared" si="4"/>
-        <v>2.0931031059290566E-3</v>
-      </c>
-      <c r="P72" s="3">
-        <f t="shared" si="5"/>
         <v>31.824141476521547</v>
       </c>
       <c r="Q72" s="33">
@@ -5776,7 +5772,7 @@
         <v>1.178016110562683</v>
       </c>
       <c r="S72" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4657091798532186E-3</v>
       </c>
       <c r="T72" s="33">
@@ -5835,11 +5831,11 @@
         <v>61.669130000000003</v>
       </c>
       <c r="O73" s="5">
+        <f t="shared" si="6"/>
+        <v>2.1178799437077682E-3</v>
+      </c>
+      <c r="P73" s="3">
         <f t="shared" si="4"/>
-        <v>2.1178799437077682E-3</v>
-      </c>
-      <c r="P73" s="3">
-        <f t="shared" si="5"/>
         <v>2.9632425235621414</v>
       </c>
       <c r="Q73" s="33">
@@ -5851,7 +5847,7 @@
         <v>1.1642184080830844</v>
       </c>
       <c r="S73" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4656748165745503E-3</v>
       </c>
       <c r="T73" s="33">
@@ -5910,11 +5906,11 @@
         <v>62.4</v>
       </c>
       <c r="O74" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0931031059290566E-3</v>
+      </c>
+      <c r="P74" s="3">
         <f t="shared" si="4"/>
-        <v>2.0931031059290566E-3</v>
-      </c>
-      <c r="P74" s="3">
-        <f t="shared" si="5"/>
         <v>48.081263486309716</v>
       </c>
       <c r="Q74" s="33">
@@ -5926,7 +5922,7 @@
         <v>1.178016110562683</v>
       </c>
       <c r="S74" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4657091798532186E-3</v>
       </c>
       <c r="T74" s="33">
@@ -5985,11 +5981,11 @@
         <v>62.748750000000001</v>
       </c>
       <c r="O75" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0365175140760038E-3</v>
+      </c>
+      <c r="P75" s="3">
         <f t="shared" si="4"/>
-        <v>2.0365175140760038E-3</v>
-      </c>
-      <c r="P75" s="3">
-        <f t="shared" si="5"/>
         <v>43.749811338276544</v>
       </c>
       <c r="Q75" s="33">
@@ -6001,7 +5997,7 @@
         <v>1.1845999746421498</v>
       </c>
       <c r="S75" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4124585955327283E-3</v>
       </c>
       <c r="T75" s="33">
@@ -6060,11 +6056,11 @@
         <v>62.4</v>
       </c>
       <c r="O76" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0931031059290566E-3</v>
+      </c>
+      <c r="P76" s="3">
         <f t="shared" si="4"/>
-        <v>2.0931031059290566E-3</v>
-      </c>
-      <c r="P76" s="3">
-        <f t="shared" si="5"/>
         <v>34.25376770658648</v>
       </c>
       <c r="Q76" s="33">
@@ -6076,7 +6072,7 @@
         <v>1.178016110562683</v>
       </c>
       <c r="S76" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4657091798532186E-3</v>
       </c>
       <c r="T76" s="33">
@@ -6135,11 +6131,11 @@
         <v>63.806420000000003</v>
       </c>
       <c r="O77" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9906989863648604E-3</v>
+      </c>
+      <c r="P77" s="3">
         <f t="shared" si="4"/>
-        <v>1.9906989863648604E-3</v>
-      </c>
-      <c r="P77" s="3">
-        <f t="shared" si="5"/>
         <v>528.99022554135308</v>
       </c>
       <c r="Q77" s="33">
@@ -6151,7 +6147,7 @@
         <v>1.2045671589315543</v>
       </c>
       <c r="S77" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.397930622293445E-3</v>
       </c>
       <c r="T77" s="33">
@@ -6210,11 +6206,11 @@
         <v>62.784979999999997</v>
       </c>
       <c r="O78" s="5">
+        <f t="shared" si="6"/>
+        <v>1.9459632108846249E-3</v>
+      </c>
+      <c r="P78" s="3">
         <f t="shared" si="4"/>
-        <v>1.9459632108846249E-3</v>
-      </c>
-      <c r="P78" s="3">
-        <f t="shared" si="5"/>
         <v>15.62754202318248</v>
       </c>
       <c r="Q78" s="33">
@@ -6226,7 +6222,7 @@
         <v>1.185283941367882</v>
       </c>
       <c r="S78" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3065189443542272E-3</v>
       </c>
       <c r="T78" s="33">
@@ -6285,11 +6281,11 @@
         <v>62.74971</v>
       </c>
       <c r="O79" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0632391928286273E-3</v>
+      </c>
+      <c r="P79" s="3">
         <f t="shared" si="4"/>
-        <v>2.0632391928286273E-3</v>
-      </c>
-      <c r="P79" s="3">
-        <f t="shared" si="5"/>
         <v>13.999612479294715</v>
       </c>
       <c r="Q79" s="33">
@@ -6301,7 +6297,7 @@
         <v>1.1846180979669279</v>
       </c>
       <c r="S79" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.444150488259468E-3</v>
       </c>
       <c r="T79" s="33">
@@ -6360,11 +6356,11 @@
         <v>62.853400000000001</v>
       </c>
       <c r="O80" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0062850491605233E-3</v>
+      </c>
+      <c r="P80" s="3">
         <f t="shared" si="4"/>
-        <v>2.0062850491605233E-3</v>
-      </c>
-      <c r="P80" s="3">
-        <f t="shared" si="5"/>
         <v>80.876855606135962</v>
       </c>
       <c r="Q80" s="33">
@@ -6376,7 +6372,7 @@
         <v>1.1865756058275727</v>
       </c>
       <c r="S80" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3806088976704495E-3</v>
       </c>
       <c r="T80" s="33">
@@ -6435,11 +6431,11 @@
         <v>62.633400000000002</v>
       </c>
       <c r="O81" s="5">
+        <f t="shared" si="6"/>
+        <v>2.0021567826948353E-3</v>
+      </c>
+      <c r="P81" s="3">
         <f t="shared" si="4"/>
-        <v>2.0021567826948353E-3</v>
-      </c>
-      <c r="P81" s="3">
-        <f t="shared" si="5"/>
         <v>267.96461830021155</v>
       </c>
       <c r="Q81" s="33">
@@ -6451,7 +6447,7 @@
         <v>1.1824223438993069</v>
       </c>
       <c r="S81" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.3673949158479223E-3</v>
       </c>
       <c r="T81" s="33">

</xml_diff>